<commit_message>
Added DataManipulator class and started to design it
</commit_message>
<xml_diff>
--- a/AbacusVariables.xlsx
+++ b/AbacusVariables.xlsx
@@ -432,14 +432,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="5.75" customWidth="1"/>
+    <col min="4" max="4" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="5.75" customWidth="1"/>
+    <col min="6" max="6" width="9.25" customWidth="1"/>
+    <col min="7" max="7" width="5.75" customWidth="1"/>
+    <col min="8" max="10" width="2.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added some prony manipulation into code base
</commit_message>
<xml_diff>
--- a/AbacusVariables.xlsx
+++ b/AbacusVariables.xlsx
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -608,35 +608,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>-26133000</v>
-      </c>
-      <c r="C21">
-        <v>2.7189999999999999</v>
-      </c>
-      <c r="D21">
-        <v>12922000</v>
-      </c>
-      <c r="E21">
-        <v>3.996</v>
-      </c>
-      <c r="F21">
-        <v>13227000</v>
-      </c>
-      <c r="G21">
-        <v>1.504</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>

</xml_diff>